<commit_message>
Deleted unecessary column from city lookup and tidied R code
</commit_message>
<xml_diff>
--- a/City Lookup.xlsx
+++ b/City Lookup.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\my documents\Medicaid claims\MedicaidRProj\PersonTable\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\My Documents\Medicaid claims\R Projects\Medicaid-PersonTable\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="210" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="166">
   <si>
     <t>city</t>
   </si>
@@ -32,9 +32,6 @@
     <t>ICU_regex</t>
   </si>
   <si>
-    <t>search_intent</t>
-  </si>
-  <si>
     <t>notes</t>
   </si>
   <si>
@@ -72,12 +69,6 @@
   </si>
   <si>
     <t>CARN[:alnum:]*ON</t>
-  </si>
-  <si>
-    <t>Anything starting ABUR</t>
-  </si>
-  <si>
-    <t>AUBxxxN or AUDxxxN (at the start)</t>
   </si>
   <si>
     <t>COVINGTON</t>
@@ -848,21 +839,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D101"/>
+  <dimension ref="A1:C101"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A30" workbookViewId="0">
-      <selection activeCell="A38" sqref="A38"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.5703125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="58.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="32.28515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="74" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -872,826 +862,817 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
+      </c>
+      <c r="B7" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
+      <c r="B10" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>91</v>
+      </c>
+      <c r="B11" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>12</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>90</v>
+      </c>
+      <c r="B13" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B14" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>13</v>
+      </c>
+      <c r="B15" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>85</v>
-      </c>
-      <c r="B8" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>91</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>94</v>
-      </c>
-      <c r="B11" t="s">
-        <v>140</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>93</v>
-      </c>
-      <c r="B13" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" t="s">
-        <v>99</v>
-      </c>
-      <c r="B14" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
-        <v>14</v>
-      </c>
-      <c r="B15" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>18</v>
-      </c>
-      <c r="B16" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="B18" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="B19" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
+        <v>18</v>
+      </c>
+      <c r="B22" t="s">
         <v>21</v>
-      </c>
-      <c r="B22" t="s">
-        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B23" t="s">
-        <v>25</v>
+        <v>22</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="B24" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="B25" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B26" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>30</v>
+      </c>
+      <c r="B32" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
+        <v>30</v>
+      </c>
+      <c r="B33" t="s">
         <v>33</v>
       </c>
-      <c r="B32" t="s">
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>30</v>
+      </c>
+      <c r="B34" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>103</v>
+      </c>
+      <c r="B35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
+        <v>151</v>
+      </c>
+      <c r="B36" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
+        <v>161</v>
+      </c>
+      <c r="B37" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>161</v>
+      </c>
+      <c r="B38" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
-        <v>33</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="B39" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>33</v>
-      </c>
-      <c r="B34" t="s">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
+        <v>35</v>
+      </c>
+      <c r="B40" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
+        <v>41</v>
+      </c>
+      <c r="B41" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" t="s">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>40</v>
+      </c>
+      <c r="C43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" t="s">
+        <v>43</v>
+      </c>
+      <c r="B45" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>43</v>
+      </c>
+      <c r="B47" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" t="s">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>49</v>
+      </c>
+      <c r="B49" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>107</v>
+      </c>
+      <c r="B50" t="s">
         <v>106</v>
       </c>
-      <c r="B35" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>108</v>
+      </c>
+      <c r="B51" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
         <v>154</v>
       </c>
-      <c r="B36" t="s">
+      <c r="B52" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>110</v>
+      </c>
+      <c r="B53" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>111</v>
+      </c>
+      <c r="B54" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>113</v>
+      </c>
+      <c r="B55" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>51</v>
+      </c>
+      <c r="B56" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>51</v>
+      </c>
+      <c r="B57" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
-        <v>164</v>
-      </c>
-      <c r="B37" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
-        <v>164</v>
-      </c>
-      <c r="B38" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
-        <v>38</v>
-      </c>
-      <c r="B39" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
-        <v>38</v>
-      </c>
-      <c r="B40" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>44</v>
-      </c>
-      <c r="B41" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
-        <v>44</v>
-      </c>
-      <c r="B42" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>44</v>
-      </c>
-      <c r="B43" t="s">
-        <v>43</v>
-      </c>
-      <c r="D43" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>46</v>
-      </c>
-      <c r="B44" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
-        <v>46</v>
-      </c>
-      <c r="B45" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
-        <v>46</v>
-      </c>
-      <c r="B46" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
-        <v>46</v>
-      </c>
-      <c r="B47" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>115</v>
+      </c>
+      <c r="B58" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>117</v>
+      </c>
+      <c r="B59" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
         <v>52</v>
       </c>
-      <c r="B49" t="s">
+      <c r="B60" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>52</v>
+      </c>
+      <c r="B61" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>110</v>
-      </c>
-      <c r="B50" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>111</v>
-      </c>
-      <c r="B51" t="s">
+      <c r="B62" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>53</v>
+      </c>
+      <c r="B63" t="s">
+        <v>55</v>
+      </c>
+      <c r="C63" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>119</v>
+      </c>
+      <c r="B64" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>159</v>
+      </c>
+      <c r="B65" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>120</v>
+      </c>
+      <c r="B66" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>157</v>
-      </c>
-      <c r="B52" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
-        <v>113</v>
-      </c>
-      <c r="B53" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>114</v>
-      </c>
-      <c r="B54" t="s">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>121</v>
+      </c>
+      <c r="B67" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>122</v>
+      </c>
+      <c r="B68" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>116</v>
-      </c>
-      <c r="B55" t="s">
-        <v>115</v>
-      </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>54</v>
-      </c>
-      <c r="B56" t="s">
-        <v>159</v>
-      </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>54</v>
-      </c>
-      <c r="B57" t="s">
-        <v>158</v>
-      </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>118</v>
-      </c>
-      <c r="B58" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>120</v>
-      </c>
-      <c r="B59" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>55</v>
-      </c>
-      <c r="B60" t="s">
-        <v>160</v>
-      </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>55</v>
-      </c>
-      <c r="B61" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>56</v>
-      </c>
-      <c r="B62" t="s">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>122</v>
+      </c>
+      <c r="B69" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" t="s">
+        <v>95</v>
+      </c>
+      <c r="B70" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A71" t="s">
+        <v>95</v>
+      </c>
+      <c r="B71" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A72" t="s">
+        <v>95</v>
+      </c>
+      <c r="B72" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A73" t="s">
+        <v>127</v>
+      </c>
+      <c r="B73" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" t="s">
         <v>57</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>56</v>
-      </c>
-      <c r="B63" t="s">
+      <c r="B74" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" t="s">
         <v>58</v>
       </c>
-      <c r="D63" t="s">
+      <c r="B75" t="s">
         <v>59</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>122</v>
-      </c>
-      <c r="B64" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>162</v>
-      </c>
-      <c r="B65" t="s">
-        <v>161</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>123</v>
-      </c>
-      <c r="B66" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
-        <v>124</v>
-      </c>
-      <c r="B67" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
-        <v>125</v>
-      </c>
-      <c r="B68" t="s">
-        <v>148</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
-        <v>125</v>
-      </c>
-      <c r="B69" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
-        <v>98</v>
-      </c>
-      <c r="B70" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
-        <v>98</v>
-      </c>
-      <c r="B71" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
-        <v>98</v>
-      </c>
-      <c r="B72" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
-        <v>130</v>
-      </c>
-      <c r="B73" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+      <c r="C75" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" t="s">
+        <v>58</v>
+      </c>
+      <c r="B76" t="s">
         <v>60</v>
       </c>
-      <c r="B74" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
-        <v>61</v>
-      </c>
-      <c r="B75" t="s">
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" t="s">
         <v>62</v>
       </c>
-      <c r="D75" t="s">
+      <c r="B77" t="s">
+        <v>63</v>
+      </c>
+      <c r="C77" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>62</v>
+      </c>
+      <c r="B78" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>61</v>
-      </c>
-      <c r="B76" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>62</v>
+      </c>
+      <c r="B79" t="s">
         <v>65</v>
       </c>
-      <c r="B77" t="s">
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" t="s">
+        <v>62</v>
+      </c>
+      <c r="B80" t="s">
         <v>66</v>
-      </c>
-      <c r="D77" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
-        <v>65</v>
-      </c>
-      <c r="B78" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
-        <v>65</v>
-      </c>
-      <c r="B79" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
-        <v>65</v>
-      </c>
-      <c r="B80" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B81" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B82" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B83" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B84" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B85" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="B86" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B87" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B88" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B89" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="B90" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="B91" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="B92" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B93" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="B94" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
+        <v>78</v>
+      </c>
+      <c r="B95" t="s">
         <v>81</v>
-      </c>
-      <c r="B95" t="s">
-        <v>84</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B96" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B98" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="B99" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B100" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B101" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added more rows for city clean up
</commit_message>
<xml_diff>
--- a/City Lookup.xlsx
+++ b/City Lookup.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="207" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="178">
   <si>
     <t>city</t>
   </si>
@@ -41,9 +41,6 @@
     <t>BELLEVUE</t>
   </si>
   <si>
-    <t>^AU[BD][:alnum:]*N</t>
-  </si>
-  <si>
     <t>^ABUR</t>
   </si>
   <si>
@@ -146,9 +143,6 @@
     <t>AEMMORE</t>
   </si>
   <si>
-    <t>KEN</t>
-  </si>
-  <si>
     <t>KENMORE</t>
   </si>
   <si>
@@ -215,12 +209,6 @@
     <t>SEATTLE</t>
   </si>
   <si>
-    <t>ATTLE</t>
-  </si>
-  <si>
-    <t>[DS]EA[:alnum:]*[KLT]E</t>
-  </si>
-  <si>
     <t>SEATTL</t>
   </si>
   <si>
@@ -491,12 +479,6 @@
     <t>LYNNWOOD</t>
   </si>
   <si>
-    <t>MT[:alnum:]*[:space:]*[:alnum:]*AKE[:space:]*TERR</t>
-  </si>
-  <si>
-    <t>MOU[NT][:alnum:]*[:space:]*[:alnum:]*AKE[:space:]*TERR</t>
-  </si>
-  <si>
     <t>NOR[:alnum:]*[:space:]*PARK</t>
   </si>
   <si>
@@ -522,6 +504,60 @@
   </si>
   <si>
     <t>YWCA SHELTER</t>
+  </si>
+  <si>
+    <t>\\ENT</t>
+  </si>
+  <si>
+    <t>^KEN$</t>
+  </si>
+  <si>
+    <t>[.478DS]EA[:alnum:]*[KLT]E</t>
+  </si>
+  <si>
+    <t>06ATTLE</t>
+  </si>
+  <si>
+    <t>4EDERAL WAY</t>
+  </si>
+  <si>
+    <t>7UBURN</t>
+  </si>
+  <si>
+    <t>[48]ENTON</t>
+  </si>
+  <si>
+    <t>BUCKLEY</t>
+  </si>
+  <si>
+    <t>8UCKLEY</t>
+  </si>
+  <si>
+    <t>^AU[BDN][:alnum:]*N</t>
+  </si>
+  <si>
+    <t>EATTLE</t>
+  </si>
+  <si>
+    <t>SE00TLE00</t>
+  </si>
+  <si>
+    <t>MT[:alnum:]*[:space:]*[:alnum:]*AKE[:space:]*TER</t>
+  </si>
+  <si>
+    <t>MOU[NT][:alnum:]*[:space:]*[:alnum:]*AKE[:space:]*TER</t>
+  </si>
+  <si>
+    <t>UNIVERSITY PL</t>
+  </si>
+  <si>
+    <t>BONNEY LAKE</t>
+  </si>
+  <si>
+    <t>BONNEYLAKE</t>
+  </si>
+  <si>
+    <t>BONNIE LAKE</t>
   </si>
 </sst>
 </file>
@@ -839,10 +875,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C101"/>
+  <dimension ref="A1:C111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -868,7 +904,7 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>165</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
@@ -876,7 +912,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>169</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
@@ -884,7 +920,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
@@ -892,7 +928,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
@@ -900,7 +936,7 @@
         <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
@@ -908,774 +944,855 @@
         <v>3</v>
       </c>
       <c r="B7" t="s">
-        <v>84</v>
+        <v>8</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>82</v>
+        <v>3</v>
       </c>
       <c r="B8" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>88</v>
+        <v>78</v>
       </c>
       <c r="B9" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>4</v>
+        <v>84</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>83</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>91</v>
+        <v>4</v>
       </c>
       <c r="B11" t="s">
-        <v>137</v>
+        <v>9</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>87</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>133</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>90</v>
+        <v>175</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>176</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>96</v>
+        <v>175</v>
       </c>
       <c r="B14" t="s">
-        <v>138</v>
+        <v>177</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>86</v>
       </c>
       <c r="B16" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>15</v>
+        <v>167</v>
       </c>
       <c r="B17" t="s">
-        <v>17</v>
+        <v>168</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>149</v>
+        <v>92</v>
       </c>
       <c r="B18" t="s">
-        <v>150</v>
+        <v>134</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>12</v>
       </c>
       <c r="B19" t="s">
-        <v>97</v>
+        <v>13</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>18</v>
+        <v>145</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>146</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>18</v>
+        <v>94</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>99</v>
+        <v>17</v>
       </c>
       <c r="B24" t="s">
-        <v>100</v>
+        <v>18</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>101</v>
+        <v>17</v>
       </c>
       <c r="B25" t="s">
-        <v>139</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>102</v>
+        <v>17</v>
       </c>
       <c r="B26" t="s">
-        <v>140</v>
+        <v>20</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>25</v>
+        <v>17</v>
       </c>
       <c r="B27" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>25</v>
+        <v>95</v>
       </c>
       <c r="B28" t="s">
-        <v>24</v>
+        <v>96</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>26</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>135</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>28</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>136</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B31" t="s">
-        <v>31</v>
+        <v>22</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B32" t="s">
-        <v>32</v>
+        <v>23</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B33" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="B34" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>29</v>
       </c>
       <c r="B35" t="s">
-        <v>104</v>
+        <v>164</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>151</v>
+        <v>29</v>
       </c>
       <c r="B36" t="s">
-        <v>152</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="B37" t="s">
-        <v>162</v>
+        <v>31</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>161</v>
+        <v>29</v>
       </c>
       <c r="B38" t="s">
-        <v>165</v>
+        <v>32</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>35</v>
+        <v>99</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>100</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>41</v>
+        <v>147</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>148</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>156</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>41</v>
+        <v>155</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
-      </c>
-      <c r="C43" t="s">
-        <v>42</v>
+        <v>159</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B44" t="s">
-        <v>105</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>43</v>
+        <v>39</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
+        <v>39</v>
+      </c>
+      <c r="B48" t="s">
+        <v>161</v>
+      </c>
+      <c r="C48" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" t="s">
+        <v>41</v>
+      </c>
+      <c r="B49" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A51" t="s">
+        <v>41</v>
+      </c>
+      <c r="B51" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>41</v>
+      </c>
+      <c r="B52" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>41</v>
+      </c>
+      <c r="B53" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>45</v>
+      </c>
+      <c r="B54" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B55" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>103</v>
+      </c>
+      <c r="B56" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>104</v>
+      </c>
+      <c r="B57" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>106</v>
+      </c>
+      <c r="B59" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>107</v>
+      </c>
+      <c r="B60" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>109</v>
+      </c>
+      <c r="B61" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
         <v>49</v>
       </c>
-      <c r="B49" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" t="s">
-        <v>107</v>
-      </c>
-      <c r="B50" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
-        <v>108</v>
-      </c>
-      <c r="B51" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
-        <v>154</v>
-      </c>
-      <c r="B52" t="s">
-        <v>153</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+      <c r="B62" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>49</v>
+      </c>
+      <c r="B63" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>111</v>
+      </c>
+      <c r="B64" t="s">
         <v>110</v>
-      </c>
-      <c r="B53" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
-        <v>111</v>
-      </c>
-      <c r="B54" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
-        <v>113</v>
-      </c>
-      <c r="B55" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
-        <v>51</v>
-      </c>
-      <c r="B56" t="s">
-        <v>156</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
-        <v>51</v>
-      </c>
-      <c r="B57" t="s">
-        <v>155</v>
-      </c>
-    </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
-        <v>115</v>
-      </c>
-      <c r="B58" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>117</v>
-      </c>
-      <c r="B59" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
-        <v>52</v>
-      </c>
-      <c r="B60" t="s">
-        <v>157</v>
-      </c>
-    </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>52</v>
-      </c>
-      <c r="B61" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>53</v>
-      </c>
-      <c r="B62" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>53</v>
-      </c>
-      <c r="B63" t="s">
-        <v>55</v>
-      </c>
-      <c r="C63" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
-        <v>119</v>
-      </c>
-      <c r="B64" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>159</v>
+        <v>113</v>
       </c>
       <c r="B65" t="s">
-        <v>158</v>
+        <v>139</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>120</v>
+        <v>50</v>
       </c>
       <c r="B66" t="s">
-        <v>144</v>
+        <v>151</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>121</v>
+        <v>50</v>
       </c>
       <c r="B67" t="s">
-        <v>160</v>
+        <v>112</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="B68" t="s">
-        <v>145</v>
+        <v>52</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="B69" t="s">
-        <v>123</v>
+        <v>53</v>
+      </c>
+      <c r="C69" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="B70" t="s">
-        <v>124</v>
+        <v>114</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>95</v>
+        <v>153</v>
       </c>
       <c r="B71" t="s">
-        <v>125</v>
+        <v>152</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>95</v>
+        <v>116</v>
       </c>
       <c r="B72" t="s">
-        <v>94</v>
+        <v>140</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" t="s">
-        <v>127</v>
+        <v>117</v>
       </c>
       <c r="B73" t="s">
-        <v>126</v>
+        <v>154</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" t="s">
-        <v>57</v>
+        <v>118</v>
       </c>
       <c r="B74" t="s">
-        <v>128</v>
+        <v>141</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" t="s">
-        <v>58</v>
+        <v>118</v>
       </c>
       <c r="B75" t="s">
-        <v>59</v>
-      </c>
-      <c r="C75" t="s">
-        <v>61</v>
+        <v>119</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" t="s">
-        <v>58</v>
+        <v>91</v>
       </c>
       <c r="B76" t="s">
-        <v>60</v>
+        <v>166</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B77" t="s">
-        <v>63</v>
-      </c>
-      <c r="C77" t="s">
-        <v>73</v>
+        <v>120</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B78" t="s">
-        <v>64</v>
+        <v>121</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" t="s">
-        <v>62</v>
+        <v>91</v>
       </c>
       <c r="B79" t="s">
-        <v>65</v>
+        <v>90</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" t="s">
+        <v>123</v>
+      </c>
+      <c r="B80" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" t="s">
+        <v>55</v>
+      </c>
+      <c r="B81" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" t="s">
+        <v>56</v>
+      </c>
+      <c r="B82" t="s">
+        <v>57</v>
+      </c>
+      <c r="C82" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" t="s">
+        <v>56</v>
+      </c>
+      <c r="B83" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" t="s">
+        <v>60</v>
+      </c>
+      <c r="B84" t="s">
+        <v>170</v>
+      </c>
+      <c r="C84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>60</v>
+      </c>
+      <c r="B85" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>60</v>
+      </c>
+      <c r="B86" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" t="s">
+        <v>60</v>
+      </c>
+      <c r="B87" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" t="s">
+        <v>60</v>
+      </c>
+      <c r="B88" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" t="s">
+        <v>60</v>
+      </c>
+      <c r="B89" t="s">
         <v>62</v>
       </c>
-      <c r="B80" t="s">
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A90" t="s">
+        <v>60</v>
+      </c>
+      <c r="B90" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A91" t="s">
+        <v>60</v>
+      </c>
+      <c r="B91" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A92" t="s">
+        <v>60</v>
+      </c>
+      <c r="B92" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>60</v>
+      </c>
+      <c r="B93" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="81" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
-        <v>62</v>
-      </c>
-      <c r="B81" t="s">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>60</v>
+      </c>
+      <c r="B94" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="82" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>62</v>
-      </c>
-      <c r="B82" t="s">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A95" t="s">
+        <v>60</v>
+      </c>
+      <c r="B95" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>62</v>
-      </c>
-      <c r="B83" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="84" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>62</v>
-      </c>
-      <c r="B84" t="s">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A96" t="s">
         <v>70</v>
       </c>
-    </row>
-    <row r="85" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
-        <v>62</v>
-      </c>
-      <c r="B85" t="s">
+      <c r="B96" t="s">
         <v>71</v>
-      </c>
-    </row>
-    <row r="86" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
-        <v>62</v>
-      </c>
-      <c r="B86" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="87" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
-        <v>74</v>
-      </c>
-      <c r="B87" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="88" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
-        <v>131</v>
-      </c>
-      <c r="B88" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="89" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
-        <v>131</v>
-      </c>
-      <c r="B89" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="90" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
-        <v>129</v>
-      </c>
-      <c r="B90" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="91" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>76</v>
-      </c>
-      <c r="B91" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="92" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>133</v>
-      </c>
-      <c r="B92" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="93" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
-        <v>78</v>
-      </c>
-      <c r="B93" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="94" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
-        <v>78</v>
-      </c>
-      <c r="B94" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="95" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
-        <v>78</v>
-      </c>
-      <c r="B95" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="96" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
-        <v>134</v>
-      </c>
-      <c r="B96" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B97" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>86</v>
+        <v>127</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>128</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>86</v>
+        <v>125</v>
       </c>
       <c r="B99" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>93</v>
+        <v>72</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>73</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>93</v>
+        <v>129</v>
       </c>
       <c r="B101" t="s">
-        <v>164</v>
+        <v>143</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A102" t="s">
+        <v>74</v>
+      </c>
+      <c r="B102" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A103" t="s">
+        <v>74</v>
+      </c>
+      <c r="B103" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" t="s">
+        <v>74</v>
+      </c>
+      <c r="B104" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A105" t="s">
+        <v>130</v>
+      </c>
+      <c r="B105" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A106" t="s">
+        <v>130</v>
+      </c>
+      <c r="B106" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A107" t="s">
+        <v>132</v>
+      </c>
+      <c r="B107" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A108" t="s">
+        <v>82</v>
+      </c>
+      <c r="B108" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A109" t="s">
+        <v>82</v>
+      </c>
+      <c r="B109" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A110" t="s">
+        <v>89</v>
+      </c>
+      <c r="B110" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A111" t="s">
+        <v>89</v>
+      </c>
+      <c r="B111" t="s">
+        <v>158</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>